<commit_message>
Cập nhật logic xử lý báo cáo Sơn Tây (TB Ngưng PSC lũy kế năm 4.6), dọn dẹp import và đồng bộ hàm gọi trong baocaohanoi.py
</commit_message>
<xml_diff>
--- a/du_lieu_tham_chieu/LOAI_TRU_C1.5.xlsx
+++ b/du_lieu_tham_chieu/LOAI_TRU_C1.5.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,9 +407,14 @@
         <v>HDTB_ID</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>